<commit_message>
added an endpoint that allows to check which indexes are currently in use
</commit_message>
<xml_diff>
--- a/src/main/resources/Sales.xlsx
+++ b/src/main/resources/Sales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.sembrat.MCCAMBRIDGEGRP\Desktop\Do Bazy H2 MassBalanceCalculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.sembrat.MCCAMBRIDGEGRP\Desktop\Do Bazy H2 MassBalanceCalculator\Nowy folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA358FDF-D8A0-42FB-AB86-98BB1FA216D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B90399A-00E6-4CC3-A6B6-1491159D49E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="244">
   <si>
     <t>Nr_Mag</t>
   </si>
@@ -64,78 +64,18 @@
     <t>WartoscNetto</t>
   </si>
   <si>
-    <t>34P01000</t>
-  </si>
-  <si>
-    <t>Skrobia ziemniaczana</t>
-  </si>
-  <si>
     <t>KG</t>
   </si>
   <si>
-    <t>35I00616</t>
-  </si>
-  <si>
-    <t>Wkład papierowy do pieczenia WYŁOŻENIE 411x156x73</t>
-  </si>
-  <si>
-    <t>34P00132</t>
-  </si>
-  <si>
-    <t>Mąka ryżowa</t>
-  </si>
-  <si>
-    <t>34P01600</t>
-  </si>
-  <si>
-    <t>Glicerol</t>
-  </si>
-  <si>
-    <t>34D05110</t>
-  </si>
-  <si>
-    <t>Blendesi Free Range</t>
-  </si>
-  <si>
-    <t>34D01324</t>
-  </si>
-  <si>
-    <t>Wiśnie połówki i całe JASNOCZERWONE</t>
-  </si>
-  <si>
-    <t>34D01867</t>
-  </si>
-  <si>
-    <t>Posypka Permafrost (Palm Free)</t>
-  </si>
-  <si>
-    <t>34D02477</t>
-  </si>
-  <si>
-    <t>Nadzienie Lemon Curd Sainsbury's 58037</t>
-  </si>
-  <si>
-    <t>34D02473</t>
-  </si>
-  <si>
-    <t>Nadzienie truskawka tarty Sainsbury (MP585/MP540)</t>
-  </si>
-  <si>
     <t>1000</t>
   </si>
   <si>
     <t>22R00019</t>
   </si>
   <si>
-    <t>Tesco Ms Molly's Jumbo Straw &amp; Van SR*12 RSPO-SG</t>
-  </si>
-  <si>
     <t>SZT</t>
   </si>
   <si>
-    <t>22R00020</t>
-  </si>
-  <si>
     <t>Tesco Ms Molly's Raspberry SR *12 (RSPO-SG)</t>
   </si>
   <si>
@@ -145,12 +85,6 @@
     <t>Tesco 6 Assorted Jam Tarts *12 '2008  (RSPO-SG)</t>
   </si>
   <si>
-    <t>22M00111</t>
-  </si>
-  <si>
-    <t>Tesco Princess Celebration Cake New *2 (RSPO-SG)</t>
-  </si>
-  <si>
     <t>22M00167</t>
   </si>
   <si>
@@ -169,12 +103,6 @@
     <t>JS 6 Assorted Jam Tarts *12 (RSPO-SG)</t>
   </si>
   <si>
-    <t>22N00003</t>
-  </si>
-  <si>
-    <t>Iceland Standard Iced Bar 400g *12</t>
-  </si>
-  <si>
     <t>22T00250</t>
   </si>
   <si>
@@ -193,12 +121,6 @@
     <t>Morrisons 6 Assorted Jam tarts *12 (RSPO-SG)</t>
   </si>
   <si>
-    <t>22R00109</t>
-  </si>
-  <si>
-    <t>Morrisons Raspberry Swiss Roll *12  (RSP0-SG)</t>
-  </si>
-  <si>
     <t>800.000</t>
   </si>
   <si>
@@ -319,12 +241,6 @@
     <t>1054.170</t>
   </si>
   <si>
-    <t>22C08078</t>
-  </si>
-  <si>
-    <t>Aldi Triple Chocolate Swiss Roll*12 (RSPO-SG;RA-MB)</t>
-  </si>
-  <si>
     <t>198.000</t>
   </si>
   <si>
@@ -335,6 +251,510 @@
   </si>
   <si>
     <t>Nazwa 2</t>
+  </si>
+  <si>
+    <t>22C00103</t>
+  </si>
+  <si>
+    <t>Tesco Birthday Cube Cake *2 (RSPO-SG;RA-MB)</t>
+  </si>
+  <si>
+    <t>22C00125</t>
+  </si>
+  <si>
+    <t>Morrison SIWC - 15 Party Cubes *2 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C00138</t>
+  </si>
+  <si>
+    <t>Asda Birthday Cube Cake *2 (RSPO-SG; RA -MB)</t>
+  </si>
+  <si>
+    <t>22C00139</t>
+  </si>
+  <si>
+    <t>Waitrose Happy Birthday Cubes *2 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C00141</t>
+  </si>
+  <si>
+    <t>Tesco 6 Easter Cubes 2023*8 (RSPO-SG; RA-MB)</t>
+  </si>
+  <si>
+    <t>22C04733</t>
+  </si>
+  <si>
+    <t>Perfetto Torcik Jaffa 38g*40 (RSPO-MB, RA-MB)</t>
+  </si>
+  <si>
+    <t>22C04734</t>
+  </si>
+  <si>
+    <t>Biscotto Torcik czekoladowy 38g*40 (RSPO-MB; RA-MB)</t>
+  </si>
+  <si>
+    <t>22C08049</t>
+  </si>
+  <si>
+    <t>Aldi 5 Raspberry Mini Rolls *12 (RSPO-SG;RA-MB)</t>
+  </si>
+  <si>
+    <t>22C08082</t>
+  </si>
+  <si>
+    <t>Hoppers 10 Choco Mini rolls *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C08085</t>
+  </si>
+  <si>
+    <t>Hoppers 8 Chocolate Nom Noms *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C08107</t>
+  </si>
+  <si>
+    <t>Sainsbury 5 Mini Wiggles Cake *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C08122</t>
+  </si>
+  <si>
+    <t>Aldi Cuthbert Caterpillar Cake *6 (RSPO-SG;RA-MB)</t>
+  </si>
+  <si>
+    <t>22C08129</t>
+  </si>
+  <si>
+    <t>Aldi Jaffa&amp;Titan Cake Bars*14 (RSPO-SG; RA-MB)</t>
+  </si>
+  <si>
+    <t>22C08130</t>
+  </si>
+  <si>
+    <t>Aldi Choceur&amp;Dreamy Cake Bars *14 (RSPO-SG; RA-MB)</t>
+  </si>
+  <si>
+    <t>22C08131</t>
+  </si>
+  <si>
+    <t>Aldi Beverley Manor 6 Strawberry Mini Rolls *14 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C08132</t>
+  </si>
+  <si>
+    <t>Sainsbury 5 Easter Mini Rolls *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C08133</t>
+  </si>
+  <si>
+    <t>Aldi Cuthbert Caterpillar Cake *4 (RSPO-SG; RA-MB)</t>
+  </si>
+  <si>
+    <t>22C09014</t>
+  </si>
+  <si>
+    <t>Cabico 6 Lemon Mini Rolls 12*150g (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C09016</t>
+  </si>
+  <si>
+    <t>Cabico 6 Strawberry Mini Rolls 12*150g (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C20033</t>
+  </si>
+  <si>
+    <t>Hoppe Mandemakers 5 Str MR white dec *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C20034</t>
+  </si>
+  <si>
+    <t>Hoppe 6 Straw MR choc dec 150g*12 VOS04 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C20035</t>
+  </si>
+  <si>
+    <t>Hoppe 6 MR straw choc dec 150g*12 GK010 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C20036</t>
+  </si>
+  <si>
+    <t>Hoppe 6 Mini Yoghurt Cherry Deco roll *12 (GK011) (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C20037</t>
+  </si>
+  <si>
+    <t>Hoppe 6 Mini rolls chocolade deco 150g*12 (VOS05) (RSPO-MB)</t>
+  </si>
+  <si>
+    <t>22C20038</t>
+  </si>
+  <si>
+    <t>Hoppe 6 MR Strawberry *12 HO167 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C20040</t>
+  </si>
+  <si>
+    <t>Hoppe 5 MR Chocolate deco 125g*12(GK012) (RSPO-MB)</t>
+  </si>
+  <si>
+    <t>22C20043</t>
+  </si>
+  <si>
+    <t>Hoppe 6 MR Raspberry pink deco 12x6 (VOS06) (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22C20049</t>
+  </si>
+  <si>
+    <t>Hoppe CakeRolletje Framb 150g *12 DK001 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22M00173</t>
+  </si>
+  <si>
+    <t>Tesco Princess Cake 2023 *2 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22M00174</t>
+  </si>
+  <si>
+    <t>Tesco Rose Bouquet Cake *2 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22M00175</t>
+  </si>
+  <si>
+    <t>Tesco Carrot Celebration Cake *2 (RSPO-SG; RA-MB)</t>
+  </si>
+  <si>
+    <t>Tesco Ms Molly's Jumbo Straw &amp; Van SR (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R00112</t>
+  </si>
+  <si>
+    <t>Morrisons Jumbo Strawb. &amp; Vanilla SR *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R00113</t>
+  </si>
+  <si>
+    <t>Morrisons Jumbo Choco. &amp; Vanilla SR *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01211</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Rasber&amp;Cream R (6*300g) (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01212</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Strawb&amp;Cream R (6*300g) (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01213</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Lemon&amp;Cream R (6*300 g) (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01214</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Cocoa&amp;Cream R (6*300g) (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01221</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Rasp&amp;Cream(6*300g) 1GBP (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01222</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Straw&amp;Cream(6*300g) 1GBP (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01223</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Lemon&amp;Cream(6*300g) 1GBP (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01224</t>
+  </si>
+  <si>
+    <t>Rolada Cabico Cocoa&amp;Cream(6*300g) 1GBP (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22R01401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sainsbury Jumbo Strawberry Swiss Roll (12*365g) (RSPO-SG) </t>
+  </si>
+  <si>
+    <t>22R01402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sainsbury Jumbo Chocolate Swiss Roll (12*365g) (RSPO-SG) </t>
+  </si>
+  <si>
+    <t>22T00101</t>
+  </si>
+  <si>
+    <t>Aldi Holly Lane 6 Assorted Jam Tart *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22T00207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Stop 6 Assorted Jam tarts*12 </t>
+  </si>
+  <si>
+    <t>22T00220</t>
+  </si>
+  <si>
+    <t>Morrisons 6 Strawberry Jam tarts *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22T00221</t>
+  </si>
+  <si>
+    <t>Morrisons 6 Lemon Curd Jam tarts *12 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22T00252</t>
+  </si>
+  <si>
+    <t>Hoppers 9 Assorted JT Non - Price *16 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22T00411</t>
+  </si>
+  <si>
+    <t>Tesco 6 Lemon Curd Tarts *12  `2008 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22T00420</t>
+  </si>
+  <si>
+    <t>Hoppers 9 Lemon Curd Tarts (RSPO-SG) *16</t>
+  </si>
+  <si>
+    <t>22T10137</t>
+  </si>
+  <si>
+    <t>Booker 6 Assorted Jam tarts *6 (RSPO-SG)</t>
+  </si>
+  <si>
+    <t>22T10262</t>
+  </si>
+  <si>
+    <t>Hoppers 6 Assorted Jam Tarts *12 (RSPO-SG) dla Iceland</t>
+  </si>
+  <si>
+    <t>22T10263</t>
+  </si>
+  <si>
+    <t>Hoppers 6 Assorted Jam Tarts *12 dla Freemans</t>
+  </si>
+  <si>
+    <t>FG040215</t>
+  </si>
+  <si>
+    <t>FG040217</t>
+  </si>
+  <si>
+    <t>Tesco Ms Molly's Jumbo Choc&amp;Van SR (RSPO-SG;RA-MB)</t>
+  </si>
+  <si>
+    <t>224.001</t>
+  </si>
+  <si>
+    <t>524.161</t>
+  </si>
+  <si>
+    <t>198.001</t>
+  </si>
+  <si>
+    <t>641.521</t>
+  </si>
+  <si>
+    <t>224.002</t>
+  </si>
+  <si>
+    <t>524.162</t>
+  </si>
+  <si>
+    <t>198.002</t>
+  </si>
+  <si>
+    <t>641.522</t>
+  </si>
+  <si>
+    <t>224.003</t>
+  </si>
+  <si>
+    <t>524.163</t>
+  </si>
+  <si>
+    <t>198.003</t>
+  </si>
+  <si>
+    <t>641.523</t>
+  </si>
+  <si>
+    <t>224.004</t>
+  </si>
+  <si>
+    <t>524.164</t>
+  </si>
+  <si>
+    <t>198.004</t>
+  </si>
+  <si>
+    <t>641.524</t>
+  </si>
+  <si>
+    <t>224.005</t>
+  </si>
+  <si>
+    <t>524.165</t>
+  </si>
+  <si>
+    <t>198.005</t>
+  </si>
+  <si>
+    <t>641.525</t>
+  </si>
+  <si>
+    <t>224.006</t>
+  </si>
+  <si>
+    <t>524.166</t>
+  </si>
+  <si>
+    <t>198.006</t>
+  </si>
+  <si>
+    <t>641.526</t>
+  </si>
+  <si>
+    <t>224.007</t>
+  </si>
+  <si>
+    <t>524.167</t>
+  </si>
+  <si>
+    <t>198.007</t>
+  </si>
+  <si>
+    <t>641.527</t>
+  </si>
+  <si>
+    <t>224.008</t>
+  </si>
+  <si>
+    <t>524.168</t>
+  </si>
+  <si>
+    <t>198.008</t>
+  </si>
+  <si>
+    <t>641.528</t>
+  </si>
+  <si>
+    <t>224.009</t>
+  </si>
+  <si>
+    <t>524.169</t>
+  </si>
+  <si>
+    <t>198.009</t>
+  </si>
+  <si>
+    <t>641.529</t>
+  </si>
+  <si>
+    <t>224.010</t>
+  </si>
+  <si>
+    <t>524.170</t>
+  </si>
+  <si>
+    <t>198.010</t>
+  </si>
+  <si>
+    <t>641.530</t>
+  </si>
+  <si>
+    <t>224.011</t>
+  </si>
+  <si>
+    <t>524.171</t>
+  </si>
+  <si>
+    <t>198.011</t>
+  </si>
+  <si>
+    <t>641.531</t>
+  </si>
+  <si>
+    <t>224.012</t>
+  </si>
+  <si>
+    <t>524.172</t>
+  </si>
+  <si>
+    <t>198.012</t>
+  </si>
+  <si>
+    <t>641.532</t>
+  </si>
+  <si>
+    <t>224.013</t>
+  </si>
+  <si>
+    <t>524.173</t>
+  </si>
+  <si>
+    <t>198.013</t>
+  </si>
+  <si>
+    <t>641.533</t>
+  </si>
+  <si>
+    <t>224.014</t>
+  </si>
+  <si>
+    <t>524.174</t>
+  </si>
+  <si>
+    <t>198.014</t>
+  </si>
+  <si>
+    <t>641.534</t>
+  </si>
+  <si>
+    <t>224.015</t>
+  </si>
+  <si>
+    <t>524.175</t>
   </si>
 </sst>
 </file>
@@ -682,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56D5AC1-56E9-4CD3-94CA-758B4151595F}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,13 +1159,13 @@
         <v>2832</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D2">
         <v>2835</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>44645</v>
@@ -754,19 +1174,19 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="M2">
         <v>3168</v>
@@ -780,13 +1200,13 @@
         <v>2832</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D3">
         <v>2835</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>44659</v>
@@ -795,19 +1215,19 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="M3">
         <v>3575.1</v>
@@ -821,13 +1241,13 @@
         <v>2832</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D4">
         <v>2835</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F4">
         <v>44652</v>
@@ -836,19 +1256,19 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="M4">
         <v>3168</v>
@@ -862,13 +1282,13 @@
         <v>2832</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D5">
         <v>2835</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F5">
         <v>44673</v>
@@ -877,19 +1297,19 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="M5">
         <v>7920</v>
@@ -903,13 +1323,13 @@
         <v>2832</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>2835</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F6">
         <v>44708</v>
@@ -918,19 +1338,19 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="M6">
         <v>68000</v>
@@ -944,13 +1364,13 @@
         <v>2832</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D7">
         <v>2835</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F7">
         <v>44631</v>
@@ -959,19 +1379,19 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="M7">
         <v>3620</v>
@@ -985,13 +1405,13 @@
         <v>2832</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>2835</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>44515</v>
@@ -1000,19 +1420,19 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="L8" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="M8">
         <v>6063.75</v>
@@ -1026,13 +1446,13 @@
         <v>2832</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>2835</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F9">
         <v>44510</v>
@@ -1041,19 +1461,19 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="M9">
         <v>9880</v>
@@ -1067,13 +1487,13 @@
         <v>2832</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>2835</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F10">
         <v>44510</v>
@@ -1082,19 +1502,19 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="M10">
         <v>4158</v>
@@ -1108,13 +1528,13 @@
         <v>2832</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D11">
         <v>2835</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F11">
         <v>44459</v>
@@ -1123,19 +1543,19 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="L11" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1149,13 +1569,13 @@
         <v>2832</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D12">
         <v>2835</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F12">
         <v>44429</v>
@@ -1164,19 +1584,19 @@
         <v>4</v>
       </c>
       <c r="H12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" t="s">
         <v>13</v>
       </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1190,13 +1610,13 @@
         <v>2832</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D13">
         <v>2835</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F13">
         <v>44428</v>
@@ -1205,19 +1625,19 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" t="s">
         <v>13</v>
       </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" t="s">
-        <v>15</v>
-      </c>
       <c r="K13" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="L13" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="M13">
         <v>6380</v>
@@ -1231,13 +1651,13 @@
         <v>2832</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D14">
         <v>2835</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F14">
         <v>44435</v>
@@ -1246,19 +1666,19 @@
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="I14" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="M14">
         <v>6074.76</v>
@@ -1272,13 +1692,13 @@
         <v>2832</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D15">
         <v>2835</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F15">
         <v>44435</v>
@@ -1287,19 +1707,19 @@
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="L15" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="M15">
         <v>6185.5</v>
@@ -1313,13 +1733,13 @@
         <v>2832</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D16">
         <v>2835</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F16">
         <v>44419</v>
@@ -1328,19 +1748,19 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" t="s">
         <v>13</v>
       </c>
-      <c r="I16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" t="s">
-        <v>15</v>
-      </c>
       <c r="K16" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="M16">
         <v>3190</v>
@@ -1354,13 +1774,13 @@
         <v>2832</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D17">
         <v>2835</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F17">
         <v>44456</v>
@@ -1369,19 +1789,19 @@
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
       <c r="I17" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K17" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="L17" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="M17">
         <v>9791.1</v>
@@ -1395,13 +1815,13 @@
         <v>2832</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D18">
         <v>2835</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F18">
         <v>44418</v>
@@ -1410,19 +1830,19 @@
         <v>4</v>
       </c>
       <c r="H18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" t="s">
         <v>13</v>
       </c>
-      <c r="I18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" t="s">
-        <v>15</v>
-      </c>
       <c r="K18" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="L18" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="M18">
         <v>1196.25</v>
@@ -1436,13 +1856,13 @@
         <v>2832</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D19">
         <v>2838</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F19">
         <v>44418</v>
@@ -1451,19 +1871,19 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="I19" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="J19" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K19" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="M19">
         <v>14704.2</v>
@@ -1477,13 +1897,13 @@
         <v>2832</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D20">
         <v>2838</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F20">
         <v>44418</v>
@@ -1492,19 +1912,19 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="J20" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="L20" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="M20">
         <v>3895.36</v>
@@ -1518,13 +1938,13 @@
         <v>2832</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D21">
         <v>2838</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F21">
         <v>44418</v>
@@ -1533,19 +1953,19 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K21" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="L21" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="M21">
         <v>13051.2</v>
@@ -1559,13 +1979,13 @@
         <v>2832</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D22">
         <v>2838</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F22">
         <v>44418</v>
@@ -1574,19 +1994,19 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="I22" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="J22" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K22" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="L22" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="M22">
         <v>13422</v>
@@ -1600,13 +2020,13 @@
         <v>2832</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D23">
         <v>2838</v>
       </c>
       <c r="E23" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F23">
         <v>44418</v>
@@ -1615,19 +2035,19 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="I23" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="J23" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K23" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="L23" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="M23">
         <v>11246.4</v>
@@ -1641,13 +2061,13 @@
         <v>2832</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D24">
         <v>2838</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F24">
         <v>44418</v>
@@ -1656,19 +2076,19 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="I24" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="J24" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K24" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="L24" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="M24">
         <v>11129.6</v>
@@ -1682,13 +2102,13 @@
         <v>2832</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D25">
         <v>2838</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F25">
         <v>44418</v>
@@ -1697,19 +2117,19 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="I25" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="J25" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="L25" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="M25">
         <v>10285.799999999999</v>
@@ -1723,13 +2143,13 @@
         <v>2832</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D26">
         <v>2838</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F26">
         <v>44418</v>
@@ -1738,19 +2158,19 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="I26" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="J26" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="L26" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="M26">
         <v>162483.29999999999</v>
@@ -1764,13 +2184,13 @@
         <v>2832</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D27">
         <v>2838</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F27">
         <v>44418</v>
@@ -1779,19 +2199,19 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="J27" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K27" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="L27" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="M27">
         <v>7599.43</v>
@@ -1805,13 +2225,13 @@
         <v>2832</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D28">
         <v>2838</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F28">
         <v>44418</v>
@@ -1820,19 +2240,19 @@
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="I28" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="J28" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K28" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="L28" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="M28">
         <v>5657.4</v>
@@ -1846,13 +2266,13 @@
         <v>2832</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D29">
         <v>2838</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F29">
         <v>44418</v>
@@ -1861,19 +2281,19 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="I29" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="J29" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K29" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="L29" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="M29">
         <v>16869.599999999999</v>
@@ -1887,13 +2307,13 @@
         <v>2832</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D30">
         <v>2838</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F30">
         <v>44418</v>
@@ -1902,19 +2322,19 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="J30" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="L30" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="M30">
         <v>16694.400000000001</v>
@@ -1928,13 +2348,13 @@
         <v>2832</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D31">
         <v>2838</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F31">
         <v>44418</v>
@@ -1943,19 +2363,19 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I31" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="J31" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K31" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="L31" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="M31">
         <v>10285.799999999999</v>
@@ -1969,13 +2389,13 @@
         <v>2832</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D32">
         <v>2838</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F32">
         <v>44418</v>
@@ -1984,19 +2404,19 @@
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I32" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="J32" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K32" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="L32" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M32">
         <v>13230.22</v>
@@ -2010,13 +2430,13 @@
         <v>2832</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D33">
         <v>2838</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F33">
         <v>44418</v>
@@ -2025,19 +2445,19 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="I33" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
       <c r="J33" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K33" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="L33" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="M33">
         <v>10651.41</v>
@@ -2051,13 +2471,13 @@
         <v>2832</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D34">
         <v>2838</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F34">
         <v>44418</v>
@@ -2066,19 +2486,19 @@
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="I34" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="J34" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K34" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="L34" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="M34">
         <v>3931.2</v>
@@ -2092,13 +2512,13 @@
         <v>2832</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D35">
         <v>2838</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F35">
         <v>44418</v>
@@ -2107,22 +2527,1211 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="I35" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="J35" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K35" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="L35" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="M35">
         <v>9278.2800000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>2832</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36">
+        <v>2838</v>
+      </c>
+      <c r="E36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36">
+        <v>44418</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s">
+        <v>138</v>
+      </c>
+      <c r="J36" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" t="s">
+        <v>186</v>
+      </c>
+      <c r="L36" t="s">
+        <v>187</v>
+      </c>
+      <c r="M36">
+        <v>14625.36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>2832</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37">
+        <v>2838</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37">
+        <v>44418</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37" t="s">
+        <v>139</v>
+      </c>
+      <c r="I37" t="s">
+        <v>140</v>
+      </c>
+      <c r="J37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" t="s">
+        <v>188</v>
+      </c>
+      <c r="L37" t="s">
+        <v>189</v>
+      </c>
+      <c r="M37">
+        <v>19972.439999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>2832</v>
+      </c>
+      <c r="C38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38">
+        <v>2838</v>
+      </c>
+      <c r="E38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38">
+        <v>44418</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
+        <v>141</v>
+      </c>
+      <c r="I38" t="s">
+        <v>142</v>
+      </c>
+      <c r="J38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" t="s">
+        <v>190</v>
+      </c>
+      <c r="L38" t="s">
+        <v>191</v>
+      </c>
+      <c r="M38">
+        <v>25319.52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>2832</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39">
+        <v>2838</v>
+      </c>
+      <c r="E39" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39">
+        <v>44418</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39" t="s">
+        <v>143</v>
+      </c>
+      <c r="I39" t="s">
+        <v>144</v>
+      </c>
+      <c r="J39" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" t="s">
+        <v>192</v>
+      </c>
+      <c r="L39" t="s">
+        <v>193</v>
+      </c>
+      <c r="M39">
+        <v>30666.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>2832</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40">
+        <v>2838</v>
+      </c>
+      <c r="E40" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40">
+        <v>44418</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>145</v>
+      </c>
+      <c r="I40" t="s">
+        <v>146</v>
+      </c>
+      <c r="J40" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" t="s">
+        <v>194</v>
+      </c>
+      <c r="L40" t="s">
+        <v>195</v>
+      </c>
+      <c r="M40">
+        <v>36013.68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>2832</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41">
+        <v>2838</v>
+      </c>
+      <c r="E41" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41">
+        <v>44418</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41" t="s">
+        <v>147</v>
+      </c>
+      <c r="I41" t="s">
+        <v>148</v>
+      </c>
+      <c r="J41" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" t="s">
+        <v>196</v>
+      </c>
+      <c r="L41" t="s">
+        <v>197</v>
+      </c>
+      <c r="M41">
+        <v>41360.76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>2832</v>
+      </c>
+      <c r="C42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42">
+        <v>2838</v>
+      </c>
+      <c r="E42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42">
+        <v>44418</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42" t="s">
+        <v>149</v>
+      </c>
+      <c r="I42" t="s">
+        <v>150</v>
+      </c>
+      <c r="J42" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" t="s">
+        <v>198</v>
+      </c>
+      <c r="L42" t="s">
+        <v>199</v>
+      </c>
+      <c r="M42">
+        <v>46707.839999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>2832</v>
+      </c>
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43">
+        <v>2838</v>
+      </c>
+      <c r="E43" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43">
+        <v>44418</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>151</v>
+      </c>
+      <c r="I43" t="s">
+        <v>152</v>
+      </c>
+      <c r="J43" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" t="s">
+        <v>200</v>
+      </c>
+      <c r="L43" t="s">
+        <v>201</v>
+      </c>
+      <c r="M43">
+        <v>52054.92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>2832</v>
+      </c>
+      <c r="C44" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44">
+        <v>2838</v>
+      </c>
+      <c r="E44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44">
+        <v>44418</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44" t="s">
+        <v>153</v>
+      </c>
+      <c r="I44" t="s">
+        <v>154</v>
+      </c>
+      <c r="J44" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" t="s">
+        <v>202</v>
+      </c>
+      <c r="L44" t="s">
+        <v>203</v>
+      </c>
+      <c r="M44">
+        <v>57402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>2832</v>
+      </c>
+      <c r="C45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45">
+        <v>2838</v>
+      </c>
+      <c r="E45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45">
+        <v>44418</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
+        <v>155</v>
+      </c>
+      <c r="I45" t="s">
+        <v>156</v>
+      </c>
+      <c r="J45" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" t="s">
+        <v>204</v>
+      </c>
+      <c r="L45" t="s">
+        <v>205</v>
+      </c>
+      <c r="M45">
+        <v>62749.08</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>2832</v>
+      </c>
+      <c r="C46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46">
+        <v>2838</v>
+      </c>
+      <c r="E46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46">
+        <v>44418</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" t="s">
+        <v>158</v>
+      </c>
+      <c r="J46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" t="s">
+        <v>206</v>
+      </c>
+      <c r="L46" t="s">
+        <v>207</v>
+      </c>
+      <c r="M46">
+        <v>68096.160000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>2832</v>
+      </c>
+      <c r="C47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47">
+        <v>2838</v>
+      </c>
+      <c r="E47" t="s">
+        <v>75</v>
+      </c>
+      <c r="F47">
+        <v>44418</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47" t="s">
+        <v>159</v>
+      </c>
+      <c r="I47" t="s">
+        <v>160</v>
+      </c>
+      <c r="J47" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" t="s">
+        <v>208</v>
+      </c>
+      <c r="L47" t="s">
+        <v>209</v>
+      </c>
+      <c r="M47">
+        <v>73443.240000000005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>2832</v>
+      </c>
+      <c r="C48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48">
+        <v>2838</v>
+      </c>
+      <c r="E48" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48">
+        <v>44418</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48" t="s">
+        <v>161</v>
+      </c>
+      <c r="I48" t="s">
+        <v>162</v>
+      </c>
+      <c r="J48" t="s">
+        <v>16</v>
+      </c>
+      <c r="K48" t="s">
+        <v>210</v>
+      </c>
+      <c r="L48" t="s">
+        <v>211</v>
+      </c>
+      <c r="M48">
+        <v>78790.320000000007</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>2832</v>
+      </c>
+      <c r="C49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49">
+        <v>2838</v>
+      </c>
+      <c r="E49" t="s">
+        <v>75</v>
+      </c>
+      <c r="F49">
+        <v>44418</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49" t="s">
+        <v>163</v>
+      </c>
+      <c r="I49" t="s">
+        <v>164</v>
+      </c>
+      <c r="J49" t="s">
+        <v>16</v>
+      </c>
+      <c r="K49" t="s">
+        <v>212</v>
+      </c>
+      <c r="L49" t="s">
+        <v>213</v>
+      </c>
+      <c r="M49">
+        <v>84137.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>2832</v>
+      </c>
+      <c r="C50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50">
+        <v>2838</v>
+      </c>
+      <c r="E50" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50">
+        <v>44418</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" t="s">
+        <v>16</v>
+      </c>
+      <c r="K50" t="s">
+        <v>214</v>
+      </c>
+      <c r="L50" t="s">
+        <v>215</v>
+      </c>
+      <c r="M50">
+        <v>89484.479999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>2832</v>
+      </c>
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51">
+        <v>2838</v>
+      </c>
+      <c r="E51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51">
+        <v>44418</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51" t="s">
+        <v>25</v>
+      </c>
+      <c r="J51" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" t="s">
+        <v>216</v>
+      </c>
+      <c r="L51" t="s">
+        <v>217</v>
+      </c>
+      <c r="M51">
+        <v>94831.56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>2832</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52">
+        <v>2838</v>
+      </c>
+      <c r="E52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52">
+        <v>44418</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52" t="s">
+        <v>165</v>
+      </c>
+      <c r="I52" t="s">
+        <v>166</v>
+      </c>
+      <c r="J52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K52" t="s">
+        <v>218</v>
+      </c>
+      <c r="L52" t="s">
+        <v>219</v>
+      </c>
+      <c r="M52">
+        <v>100178.64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>2832</v>
+      </c>
+      <c r="C53" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53">
+        <v>2838</v>
+      </c>
+      <c r="E53" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53">
+        <v>44418</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53" t="s">
+        <v>167</v>
+      </c>
+      <c r="I53" t="s">
+        <v>168</v>
+      </c>
+      <c r="J53" t="s">
+        <v>16</v>
+      </c>
+      <c r="K53" t="s">
+        <v>220</v>
+      </c>
+      <c r="L53" t="s">
+        <v>221</v>
+      </c>
+      <c r="M53">
+        <v>105525.72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>2832</v>
+      </c>
+      <c r="C54" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54">
+        <v>2838</v>
+      </c>
+      <c r="E54" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54">
+        <v>44418</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54" t="s">
+        <v>169</v>
+      </c>
+      <c r="I54" t="s">
+        <v>170</v>
+      </c>
+      <c r="J54" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" t="s">
+        <v>222</v>
+      </c>
+      <c r="L54" t="s">
+        <v>223</v>
+      </c>
+      <c r="M54">
+        <v>110872.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>2832</v>
+      </c>
+      <c r="C55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55">
+        <v>2838</v>
+      </c>
+      <c r="E55" t="s">
+        <v>75</v>
+      </c>
+      <c r="F55">
+        <v>44418</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55" t="s">
+        <v>30</v>
+      </c>
+      <c r="I55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J55" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55" t="s">
+        <v>224</v>
+      </c>
+      <c r="L55" t="s">
+        <v>225</v>
+      </c>
+      <c r="M55">
+        <v>116219.88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>2832</v>
+      </c>
+      <c r="C56" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56">
+        <v>2838</v>
+      </c>
+      <c r="E56" t="s">
+        <v>75</v>
+      </c>
+      <c r="F56">
+        <v>44418</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56" t="s">
+        <v>26</v>
+      </c>
+      <c r="I56" t="s">
+        <v>27</v>
+      </c>
+      <c r="J56" t="s">
+        <v>16</v>
+      </c>
+      <c r="K56" t="s">
+        <v>226</v>
+      </c>
+      <c r="L56" t="s">
+        <v>227</v>
+      </c>
+      <c r="M56">
+        <v>121566.96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>2832</v>
+      </c>
+      <c r="C57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57">
+        <v>2838</v>
+      </c>
+      <c r="E57" t="s">
+        <v>75</v>
+      </c>
+      <c r="F57">
+        <v>44418</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57" t="s">
+        <v>171</v>
+      </c>
+      <c r="I57" t="s">
+        <v>172</v>
+      </c>
+      <c r="J57" t="s">
+        <v>16</v>
+      </c>
+      <c r="K57" t="s">
+        <v>228</v>
+      </c>
+      <c r="L57" t="s">
+        <v>229</v>
+      </c>
+      <c r="M57">
+        <v>126914.04</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>2832</v>
+      </c>
+      <c r="C58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58">
+        <v>2838</v>
+      </c>
+      <c r="E58" t="s">
+        <v>75</v>
+      </c>
+      <c r="F58">
+        <v>44418</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58" t="s">
+        <v>173</v>
+      </c>
+      <c r="I58" t="s">
+        <v>174</v>
+      </c>
+      <c r="J58" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" t="s">
+        <v>230</v>
+      </c>
+      <c r="L58" t="s">
+        <v>231</v>
+      </c>
+      <c r="M58">
+        <v>132261.12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>2832</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59">
+        <v>2838</v>
+      </c>
+      <c r="E59" t="s">
+        <v>75</v>
+      </c>
+      <c r="F59">
+        <v>44418</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59" t="s">
+        <v>175</v>
+      </c>
+      <c r="I59" t="s">
+        <v>176</v>
+      </c>
+      <c r="J59" t="s">
+        <v>16</v>
+      </c>
+      <c r="K59" t="s">
+        <v>232</v>
+      </c>
+      <c r="L59" t="s">
+        <v>233</v>
+      </c>
+      <c r="M59">
+        <v>137608.20000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>2832</v>
+      </c>
+      <c r="C60" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60">
+        <v>2838</v>
+      </c>
+      <c r="E60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60">
+        <v>44418</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>177</v>
+      </c>
+      <c r="I60" t="s">
+        <v>178</v>
+      </c>
+      <c r="J60" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" t="s">
+        <v>234</v>
+      </c>
+      <c r="L60" t="s">
+        <v>235</v>
+      </c>
+      <c r="M60">
+        <v>142955.28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>2832</v>
+      </c>
+      <c r="C61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61">
+        <v>2838</v>
+      </c>
+      <c r="E61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F61">
+        <v>44418</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61" t="s">
+        <v>179</v>
+      </c>
+      <c r="I61" t="s">
+        <v>180</v>
+      </c>
+      <c r="J61" t="s">
+        <v>16</v>
+      </c>
+      <c r="K61" t="s">
+        <v>236</v>
+      </c>
+      <c r="L61" t="s">
+        <v>237</v>
+      </c>
+      <c r="M61">
+        <v>148302.35999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>2832</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62">
+        <v>2838</v>
+      </c>
+      <c r="E62" t="s">
+        <v>75</v>
+      </c>
+      <c r="F62">
+        <v>44418</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62" t="s">
+        <v>181</v>
+      </c>
+      <c r="I62" t="s">
+        <v>182</v>
+      </c>
+      <c r="J62" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" t="s">
+        <v>238</v>
+      </c>
+      <c r="L62" t="s">
+        <v>239</v>
+      </c>
+      <c r="M62">
+        <v>153649.44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>2832</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63">
+        <v>2838</v>
+      </c>
+      <c r="E63" t="s">
+        <v>75</v>
+      </c>
+      <c r="F63">
+        <v>44418</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63" t="s">
+        <v>183</v>
+      </c>
+      <c r="I63" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" t="s">
+        <v>240</v>
+      </c>
+      <c r="L63" t="s">
+        <v>241</v>
+      </c>
+      <c r="M63">
+        <v>158996.51999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>2832</v>
+      </c>
+      <c r="C64" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64">
+        <v>2838</v>
+      </c>
+      <c r="E64" t="s">
+        <v>75</v>
+      </c>
+      <c r="F64">
+        <v>44418</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64" t="s">
+        <v>184</v>
+      </c>
+      <c r="I64" t="s">
+        <v>185</v>
+      </c>
+      <c r="J64" t="s">
+        <v>16</v>
+      </c>
+      <c r="K64" t="s">
+        <v>242</v>
+      </c>
+      <c r="L64" t="s">
+        <v>243</v>
+      </c>
+      <c r="M64">
+        <v>164343.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>